<commit_message>
acrescentando arquivos pentaho e atualizando scripts python de baixar e deletar csv
</commit_message>
<xml_diff>
--- a/Modelagem_dimensional.xlsx
+++ b/Modelagem_dimensional.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LVVE2K631\Documents\dados_compras_gov_federal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LVVE2K631\Documents\4.Projetos_Portifolio\dados_compras_gov_federal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97948ECC-13D0-449A-9E3E-C320FDE6D564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12616532-38E3-4664-972F-8A4209B0B92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="310" yWindow="340" windowWidth="18890" windowHeight="7360" activeTab="3" xr2:uid="{27B2CB14-3D89-4022-97B8-5FB0016979A5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="3" xr2:uid="{27B2CB14-3D89-4022-97B8-5FB0016979A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Introdução" sheetId="3" r:id="rId1"/>
@@ -979,6 +979,21 @@
     <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1014,21 +1029,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2229,32 +2229,32 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="61" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="64" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="56"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="60"/>
+      <c r="D8" s="65"/>
       <c r="H8" s="27" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="56"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="60"/>
+      <c r="D9" s="65"/>
       <c r="H9" s="10" t="s">
         <v>0</v>
       </c>
@@ -2275,11 +2275,11 @@
       <c r="A10">
         <v>4</v>
       </c>
-      <c r="B10" s="56"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="60"/>
+      <c r="D10" s="65"/>
       <c r="H10" s="19" t="s">
         <v>101</v>
       </c>
@@ -2297,11 +2297,11 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="56"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="60"/>
+      <c r="D11" s="65"/>
       <c r="H11" s="19" t="s">
         <v>100</v>
       </c>
@@ -2317,11 +2317,11 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="56"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="60"/>
+      <c r="D12" s="65"/>
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
@@ -2329,21 +2329,21 @@
       <c r="L12"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="56"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D13" s="65"/>
       <c r="H13" s="27" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="56"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="61"/>
+      <c r="D14" s="66"/>
       <c r="H14" s="10" t="s">
         <v>0</v>
       </c>
@@ -2390,13 +2390,13 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="62" t="s">
         <v>28</v>
       </c>
       <c r="C16" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="62" t="s">
+      <c r="D16" s="67" t="s">
         <v>71</v>
       </c>
       <c r="H16" s="25" t="s">
@@ -2417,18 +2417,18 @@
       <c r="A17">
         <v>6</v>
       </c>
-      <c r="B17" s="57"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="63"/>
+      <c r="D17" s="68"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="57"/>
+      <c r="B18" s="62"/>
       <c r="C18" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="64"/>
+      <c r="D18" s="69"/>
       <c r="H18" s="27" t="s">
         <v>108</v>
       </c>
@@ -2463,13 +2463,13 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="63" t="s">
         <v>34</v>
       </c>
       <c r="C20" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="65" t="s">
+      <c r="D20" s="70" t="s">
         <v>71</v>
       </c>
       <c r="H20" s="36" t="s">
@@ -2492,11 +2492,11 @@
       <c r="A21">
         <v>8</v>
       </c>
-      <c r="B21" s="58"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="66"/>
+      <c r="D21" s="71"/>
       <c r="H21" s="36" t="s">
         <v>110</v>
       </c>
@@ -2512,11 +2512,11 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="58"/>
+      <c r="B22" s="63"/>
       <c r="C22" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="67"/>
+      <c r="D22" s="72"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23">
@@ -2536,13 +2536,13 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="63" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="65" t="s">
+      <c r="D24" s="70" t="s">
         <v>71</v>
       </c>
       <c r="H24" s="10" t="s">
@@ -2565,11 +2565,11 @@
       <c r="A25">
         <v>10</v>
       </c>
-      <c r="B25" s="58"/>
+      <c r="B25" s="63"/>
       <c r="C25" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="66"/>
+      <c r="D25" s="71"/>
       <c r="H25" s="21" t="s">
         <v>113</v>
       </c>
@@ -2585,11 +2585,11 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="23" x14ac:dyDescent="0.35">
-      <c r="B26" s="58"/>
+      <c r="B26" s="63"/>
       <c r="C26" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="67"/>
+      <c r="D26" s="72"/>
       <c r="H26" s="21" t="s">
         <v>110</v>
       </c>
@@ -3184,8 +3184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFA925E-226F-41DC-9AE9-9154F11F0C5E}">
   <dimension ref="B2:J14"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3195,16 +3195,17 @@
     <col min="4" max="4" width="20.08984375" customWidth="1"/>
     <col min="6" max="6" width="24.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="70" t="s">
+      <c r="C2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="71" t="s">
+      <c r="D2" s="59" t="s">
         <v>70</v>
       </c>
       <c r="F2" s="27" t="s">
@@ -3216,13 +3217,13 @@
       <c r="J2" s="26"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="68"/>
+      <c r="D3" s="56"/>
       <c r="F3" s="10" t="s">
         <v>0</v>
       </c>
@@ -3240,11 +3241,11 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
       <c r="F4" s="25" t="s">
         <v>139</v>
       </c>
@@ -3262,11 +3263,11 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="69" t="s">
+      <c r="B5" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
       <c r="F5" s="25" t="s">
         <v>140</v>
       </c>
@@ -3282,75 +3283,75 @@
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B7" s="69" t="s">
+      <c r="B7" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="69" t="s">
+      <c r="B8" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="57"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="69" t="s">
+      <c r="B9" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="56" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="56" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="56" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B13" s="68"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>